<commit_message>
Add barcode alignment to tests
</commit_message>
<xml_diff>
--- a/tests/data/misc/barcode/report.xlsx
+++ b/tests/data/misc/barcode/report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
   <si>
     <t>CODE128</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>https://www.reportbro.com</t>
+  </si>
+  <si>
+    <t>Horizontal and vertical alignment</t>
+  </si>
+  <si>
+    <t>12345678</t>
   </si>
 </sst>
 </file>
@@ -55,12 +61,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9CB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -75,9 +87,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,13 +385,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" width="42.140625" customWidth="1"/>
+    <col min="2" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -455,6 +469,41 @@
       <c r="A15" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Add Code39 barcode for test case
</commit_message>
<xml_diff>
--- a/tests/data/misc/barcode/report.xlsx
+++ b/tests/data/misc/barcode/report.xlsx
@@ -14,7 +14,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
+  <si>
+    <t>CODE39</t>
+  </si>
+  <si>
+    <t>BARCODE</t>
+  </si>
+  <si>
+    <t>BARCODEP</t>
+  </si>
   <si>
     <t>CODE128</t>
   </si>
@@ -385,132 +394,163 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="42.140625" customWidth="1"/>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
     <col min="2" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="2"/>
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="2"/>
+      <c r="A21" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A12" r:id="rId1"/>
-    <hyperlink ref="A13" r:id="rId2"/>
-    <hyperlink ref="A14" r:id="rId3"/>
-    <hyperlink ref="A15" r:id="rId4"/>
+    <hyperlink ref="A17" r:id="rId1"/>
+    <hyperlink ref="A18" r:id="rId2"/>
+    <hyperlink ref="A19" r:id="rId3"/>
+    <hyperlink ref="A20" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>